<commit_message>
Updates to the binary template. need more test images...
</commit_message>
<xml_diff>
--- a/AxK/test-images/axk-test-images.xlsx
+++ b/AxK/test-images/axk-test-images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sampler-fs\AxK\test-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EA04AA-772A-4752-B839-953CB21F5A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83851A31-190F-40B7-ACAC-99254AF55391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
   </bookViews>
@@ -554,7 +554,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,9 +679,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="3" t="s">
         <v>26</v>
@@ -704,7 +702,9 @@
         <v>20</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
more sample images and wave files. trying to find the right SBNK structure. Not correct yet.
</commit_message>
<xml_diff>
--- a/AxK/test-images/axk-test-images.xlsx
+++ b/AxK/test-images/axk-test-images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github\sampler-fs\AxK\test-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2337B3C-378A-47AB-B2DD-14921AC4D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358153A7-43F0-48D8-B3D3-BBEA3F7194BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
   </bookViews>
   <sheets>
     <sheet name="disk images" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -118,9 +118,6 @@
     <t>File</t>
   </si>
   <si>
-    <t>sine.wav</t>
-  </si>
-  <si>
     <t>AxK Name</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>Stereo / Mono</t>
-  </si>
-  <si>
-    <t>80328 bytes</t>
   </si>
   <si>
     <t>PCM</t>
@@ -280,14 +274,129 @@
 - 1a:"SINE       1"</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>- 1a:"SINEBIG"</t>
-  </si>
-  <si>
-    <t>- 1a:"SINE" 
-- 1a:"SINEBIG"</t>
+    <t>- 1a:"SINEL"</t>
+  </si>
+  <si>
+    <t>- 1a:"SINE2" 
+- 1a:"SINEL"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4k-test-23.hds	</t>
+  </si>
+  <si>
+    <t>- 1a:"SINE2" 
+- 1a:"SINES"</t>
+  </si>
+  <si>
+    <t>3145728 bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4k-test-24.hds	</t>
+  </si>
+  <si>
+    <t>- 1a:"SINES"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4k-test-25.hds	</t>
+  </si>
+  <si>
+    <t>- 1a:"SINE2"</t>
+  </si>
+  <si>
+    <t>SINE.wav</t>
+  </si>
+  <si>
+    <t>SINE2.wav</t>
+  </si>
+  <si>
+    <t>SINE3S.wav</t>
+  </si>
+  <si>
+    <t>SINEL.wav</t>
+  </si>
+  <si>
+    <t>SINELS.wav</t>
+  </si>
+  <si>
+    <t>SINES.wav</t>
+  </si>
+  <si>
+    <t>SINE2</t>
+  </si>
+  <si>
+    <t>SINE3S</t>
+  </si>
+  <si>
+    <t>SINEL</t>
+  </si>
+  <si>
+    <t>SINELS</t>
+  </si>
+  <si>
+    <t>SINES</t>
+  </si>
+  <si>
+    <t>Stereo</t>
+  </si>
+  <si>
+    <t>WaveRIFF size</t>
+  </si>
+  <si>
+    <t>File size</t>
+  </si>
+  <si>
+    <t>Data size</t>
+  </si>
+  <si>
+    <t>882.128 bytes</t>
+  </si>
+  <si>
+    <t>1.587.628 bytes</t>
+  </si>
+  <si>
+    <t>1.323.128 bytes</t>
+  </si>
+  <si>
+    <t>352.928 bytes</t>
+  </si>
+  <si>
+    <t>88.328 bytes</t>
+  </si>
+  <si>
+    <t>88.320 bytes</t>
+  </si>
+  <si>
+    <t>88.200 bytes</t>
+  </si>
+  <si>
+    <t>352.920 bytes</t>
+  </si>
+  <si>
+    <t>882.120 bytes</t>
+  </si>
+  <si>
+    <t>352.800 bytes</t>
+  </si>
+  <si>
+    <t>1.323.120 bytes</t>
+  </si>
+  <si>
+    <t>1.323.000 bytes</t>
+  </si>
+  <si>
+    <t>1.587.720 bytes</t>
+  </si>
+  <si>
+    <t>1.587.600 bytes</t>
+  </si>
+  <si>
+    <t>882.000 bytes</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>sample wave file bigger than a 1.44mb floppy disk</t>
   </si>
 </sst>
 </file>
@@ -311,18 +420,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -374,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -386,16 +489,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -726,13 +819,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -774,29 +867,29 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -868,7 +961,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -885,15 +978,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -963,376 +1056,460 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="10">
-        <v>2</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="B23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="10">
-        <v>2</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="C24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10" t="s">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="11" t="s">
+      <c r="F26" s="9"/>
+      <c r="G26" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="10">
-        <v>2</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="10">
-        <v>2</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="10">
-        <v>1</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>77</v>
+      <c r="J26" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1343,86 +1520,300 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6C7673-437A-48C0-B697-C5422C1C405D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G3" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s">
-        <v>42</v>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all file index nodes are now parsed dynamically (for 2 file index sectors).
</commit_message>
<xml_diff>
--- a/AxK/test-images/axk-test-images.xlsx
+++ b/AxK/test-images/axk-test-images.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github\sampler-fs\AxK\test-images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.161\d\projects\github\sampler-fs\AxK\test-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358153A7-43F0-48D8-B3D3-BBEA3F7194BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B5E65-4E84-4651-921E-03CA80383391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
+    <workbookView xWindow="24390" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
   </bookViews>
   <sheets>
     <sheet name="disk images" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -348,9 +348,6 @@
     <t>Data size</t>
   </si>
   <si>
-    <t>882.128 bytes</t>
-  </si>
-  <si>
     <t>1.587.628 bytes</t>
   </si>
   <si>
@@ -372,9 +369,6 @@
     <t>352.920 bytes</t>
   </si>
   <si>
-    <t>882.120 bytes</t>
-  </si>
-  <si>
     <t>352.800 bytes</t>
   </si>
   <si>
@@ -390,13 +384,44 @@
     <t>1.587.600 bytes</t>
   </si>
   <si>
-    <t>882.000 bytes</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>sample wave file bigger than a 1.44mb floppy disk</t>
+  </si>
+  <si>
+    <t>same size as SINES, but mono</t>
+  </si>
+  <si>
+    <t>same size as SINE, but stereo</t>
+  </si>
+  <si>
+    <t>SINESM.wav</t>
+  </si>
+  <si>
+    <t>SINESM</t>
+  </si>
+  <si>
+    <t>8.948 bytes</t>
+  </si>
+  <si>
+    <t>small size for many waveforms in image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a4k-test-26.hds	</t>
+  </si>
+  <si>
+    <t>AllSamples</t>
+  </si>
+  <si>
+    <t>- 1a:"SINESM" (30x)
+- pulse 1
+- pulse 2
+- pulse 3
+- saw up
+- sine wave
+- square
+- triangle</t>
   </si>
 </sst>
 </file>
@@ -504,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,7 +545,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -819,13 +844,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1452,7 +1477,7 @@
       <c r="I24" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1480,7 +1505,7 @@
       <c r="I25" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1508,8 +1533,36 @@
       <c r="I26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="6" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1520,13 +1573,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6C7673-437A-48C0-B697-C5422C1C405D}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -1579,7 +1632,7 @@
         <v>33</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1590,13 +1643,13 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
         <v>103</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>104</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
       </c>
       <c r="F2" t="s">
         <v>34</v>
@@ -1618,6 +1671,9 @@
       </c>
       <c r="L2" t="s">
         <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1628,13 +1684,13 @@
         <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
         <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>108</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -1666,13 +1722,13 @@
         <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -1704,13 +1760,13 @@
         <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -1734,7 +1790,7 @@
         <v>40</v>
       </c>
       <c r="M5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1745,13 +1801,13 @@
         <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
@@ -1775,7 +1831,7 @@
         <v>95</v>
       </c>
       <c r="M6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1786,13 +1842,13 @@
         <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
@@ -1814,6 +1870,44 @@
       </c>
       <c r="L7" t="s">
         <v>95</v>
+      </c>
+      <c r="M7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few corrections, no new discoveries except that the node type detection is wrong.
</commit_message>
<xml_diff>
--- a/AxK/test-images/axk-test-images.xlsx
+++ b/AxK/test-images/axk-test-images.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.161\d\projects\github\sampler-fs\AxK\test-images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github\sampler-fs\AxK\test-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B5E65-4E84-4651-921E-03CA80383391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CAA11E-03A2-4D31-9689-66CD4441ACB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24390" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{18E6C213-033A-4C49-BA82-54A896297720}"/>
   </bookViews>
   <sheets>
     <sheet name="disk images" sheetId="1" r:id="rId1"/>
@@ -411,9 +411,6 @@
     <t xml:space="preserve">a4k-test-26.hds	</t>
   </si>
   <si>
-    <t>AllSamples</t>
-  </si>
-  <si>
     <t>- 1a:"SINESM" (30x)
 - pulse 1
 - pulse 2
@@ -422,6 +419,10 @@
 - sine wave
 - square
 - triangle</t>
+  </si>
+  <si>
+    <t>AllSamples
+file index is 10 sectors/5 clusters longer than a4k-test-13</t>
   </si>
 </sst>
 </file>
@@ -502,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,9 +528,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -545,7 +549,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -846,11 +850,11 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1555,14 +1559,14 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>120</v>
+      <c r="J27" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1583,7 @@
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>

</xml_diff>